<commit_message>
Prep for LS1 submission page using broker1
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testdata/TestData.xlsx
+++ b/src/main/java/com/qa/testdata/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\J Eclipes Workspace\PorchlightgroupC2Maven\src\main\java\com\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4D5FA52A-50D9-45BC-9D3B-E9EAFF535749}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FB79311E-36CE-4E9A-A0A4-4202009B0C92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8580" windowHeight="7140" activeTab="1" xr2:uid="{EB0A60BA-DB28-48EB-8C88-016B815747BD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8580" windowHeight="7140" activeTab="2" xr2:uid="{EB0A60BA-DB28-48EB-8C88-016B815747BD}"/>
   </bookViews>
   <sheets>
     <sheet name="credentials" sheetId="1" r:id="rId1"/>
-    <sheet name="aclistingdata1" sheetId="3" r:id="rId2"/>
+    <sheet name="aclistingdata" sheetId="3" r:id="rId2"/>
+    <sheet name="brokerls1data" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -509,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294CFF94-8F3F-47F6-9DE1-88B522397A2D}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,4 +588,18 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B306DF-7859-46E4-AD59-9824650113E3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>